<commit_message>
Added Find Activities Function and Modified the Weather Function
</commit_message>
<xml_diff>
--- a/ShinyWheater/R/data/activities.xlsx
+++ b/ShinyWheater/R/data/activities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matet\Desktop\ShinyWeather\ShinyWheater\R\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED4CAFEC-0F6B-4388-80EB-7BF9ACCEB8B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0158A1B-1EEC-46DD-8390-A68E7206140F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -504,10 +504,24 @@
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L28"/>
+      <selection activeCell="A31" sqref="A31:B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Added image filenames for some activities
</commit_message>
<xml_diff>
--- a/ShinyWheater/R/data/activities.xlsx
+++ b/ShinyWheater/R/data/activities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matet\Desktop\ShinyWeather\ShinyWheater\R\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0158A1B-1EEC-46DD-8390-A68E7206140F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20ACDFC3-0A3D-4340-8130-2C4B59B5ED15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="83">
   <si>
     <t>activity</t>
   </si>
@@ -96,9 +96,6 @@
     <t>sun.png</t>
   </si>
   <si>
-    <t>Walk in park</t>
-  </si>
-  <si>
     <t>ice_skating</t>
   </si>
   <si>
@@ -184,6 +181,99 @@
   </si>
   <si>
     <t>bubbles</t>
+  </si>
+  <si>
+    <t>park_walk.jpg</t>
+  </si>
+  <si>
+    <t>Walk and play the in park</t>
+  </si>
+  <si>
+    <t>https://unsplash.com/photos/yIJIO2dhWWY</t>
+  </si>
+  <si>
+    <t>ice_skating.jpg</t>
+  </si>
+  <si>
+    <t>https://unsplash.com/photos/lnCSMikKqfw</t>
+  </si>
+  <si>
+    <t>beach_picnic.jpg</t>
+  </si>
+  <si>
+    <t>https://unsplash.com/photos/hXY98KmQWkI</t>
+  </si>
+  <si>
+    <t>beach_swimming.jpg</t>
+  </si>
+  <si>
+    <t>https://unsplash.com/photos/R_BLOGXpsOg</t>
+  </si>
+  <si>
+    <t>snow_angels.jpg</t>
+  </si>
+  <si>
+    <t>https://unsplash.com/photos/_hdO_l751fE</t>
+  </si>
+  <si>
+    <t>snowman.png</t>
+  </si>
+  <si>
+    <t>https://unsplash.com/photos/5WIqleHzOok</t>
+  </si>
+  <si>
+    <t>hot_chocolate_inside.jpg</t>
+  </si>
+  <si>
+    <t>https://unsplash.com/s/photos/cozy-inside</t>
+  </si>
+  <si>
+    <t>puzzle_inside.jpg</t>
+  </si>
+  <si>
+    <t>Make a puzzle inside</t>
+  </si>
+  <si>
+    <t>https://unsplash.com/photos/AoX_1zm1NOM</t>
+  </si>
+  <si>
+    <t>biking.jpg</t>
+  </si>
+  <si>
+    <t>Go biking!</t>
+  </si>
+  <si>
+    <t>https://unsplash.com/photos/JOnaeVoNkTQ</t>
+  </si>
+  <si>
+    <t>sidewalk_drawing.jpg</t>
+  </si>
+  <si>
+    <t>Draw on the sidewalk!</t>
+  </si>
+  <si>
+    <t>https://unsplash.com/photos/erxT2em063k</t>
+  </si>
+  <si>
+    <t>water_gun_fight.jpg</t>
+  </si>
+  <si>
+    <t>Play with water guns</t>
+  </si>
+  <si>
+    <t>https://unsplash.com/photos/JSLuw23jedY</t>
+  </si>
+  <si>
+    <t>bake_cookies.jpg</t>
+  </si>
+  <si>
+    <t>Bake cookies or cakes</t>
+  </si>
+  <si>
+    <t>https://unsplash.com/photos/UyEmagArOLY</t>
+  </si>
+  <si>
+    <t>read_inside</t>
   </si>
 </sst>
 </file>
@@ -501,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:B31"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,15 +785,18 @@
         <v>20</v>
       </c>
       <c r="J5" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="K5" t="s">
-        <v>23</v>
+        <v>53</v>
+      </c>
+      <c r="L5" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6">
         <v>-20</v>
@@ -730,15 +823,18 @@
         <v>30</v>
       </c>
       <c r="J6" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="K6" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="L6" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7">
         <v>15</v>
@@ -765,15 +861,18 @@
         <v>20</v>
       </c>
       <c r="J7" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="K7" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="L7" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8">
         <v>25</v>
@@ -800,15 +899,18 @@
         <v>30</v>
       </c>
       <c r="J8" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="K8" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="L8" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9">
         <v>-15</v>
@@ -835,15 +937,18 @@
         <v>30</v>
       </c>
       <c r="J9" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
       <c r="K9" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="L9" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10">
         <v>-20</v>
@@ -870,15 +975,18 @@
         <v>20</v>
       </c>
       <c r="J10" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="K10" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="L10" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11">
         <v>-100</v>
@@ -905,15 +1013,18 @@
         <v>100</v>
       </c>
       <c r="J11" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="K11" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="L11" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12">
         <v>-100</v>
@@ -940,12 +1051,18 @@
         <v>100</v>
       </c>
       <c r="J12" t="s">
-        <v>22</v>
+        <v>67</v>
+      </c>
+      <c r="K12" t="s">
+        <v>68</v>
+      </c>
+      <c r="L12" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13">
         <v>5</v>
@@ -972,12 +1089,18 @@
         <v>25</v>
       </c>
       <c r="J13" t="s">
-        <v>22</v>
+        <v>70</v>
+      </c>
+      <c r="K13" t="s">
+        <v>71</v>
+      </c>
+      <c r="L13" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14">
         <v>20</v>
@@ -1004,12 +1127,18 @@
         <v>25</v>
       </c>
       <c r="J14" t="s">
-        <v>22</v>
+        <v>73</v>
+      </c>
+      <c r="K14" t="s">
+        <v>74</v>
+      </c>
+      <c r="L14" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15">
         <v>25</v>
@@ -1036,12 +1165,18 @@
         <v>20</v>
       </c>
       <c r="J15" t="s">
-        <v>22</v>
+        <v>76</v>
+      </c>
+      <c r="K15" t="s">
+        <v>77</v>
+      </c>
+      <c r="L15" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16">
         <v>-100</v>
@@ -1068,12 +1203,18 @@
         <v>100</v>
       </c>
       <c r="J16" t="s">
-        <v>22</v>
+        <v>79</v>
+      </c>
+      <c r="K16" t="s">
+        <v>80</v>
+      </c>
+      <c r="L16" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17">
         <v>15</v>
@@ -1105,7 +1246,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18">
         <v>15</v>
@@ -1137,7 +1278,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B19">
         <v>20</v>
@@ -1169,7 +1310,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B20">
         <v>12</v>
@@ -1201,7 +1342,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B21">
         <v>12</v>
@@ -1233,7 +1374,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -1265,7 +1406,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B23">
         <v>20</v>
@@ -1297,7 +1438,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -1329,7 +1470,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B25">
         <v>-15</v>
@@ -1361,7 +1502,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B26">
         <v>10</v>
@@ -1393,7 +1534,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B27">
         <v>10</v>
@@ -1425,7 +1566,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B28">
         <v>10</v>
@@ -1450,6 +1591,35 @@
       </c>
       <c r="I28">
         <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29">
+        <v>-100</v>
+      </c>
+      <c r="C29">
+        <v>5</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>100</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>1000</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>